<commit_message>
create analysis calendar functions
</commit_message>
<xml_diff>
--- a/back_testing/datos/calendars/calendar_usa.xlsx
+++ b/back_testing/datos/calendars/calendar_usa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravi\projects\trade_python\back_testing\datos\calendars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D398AA3-19D0-4D52-B430-A6E2FCD0CA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435C7528-A346-425A-A64D-00D9668BC0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5C8F8F81-AD8B-4CF7-B531-01F29F8E5665}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5C8F8F81-AD8B-4CF7-B531-01F29F8E5665}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="427">
   <si>
     <t>Monday, January 01, 2024</t>
   </si>
@@ -3498,6 +3498,269 @@
         <family val="2"/>
       </rPr>
       <t> for February 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Tuesday, April 01, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Job Openings and Labor Turnover Survey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for February 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Wednesday, April 02, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Occupational Employment and Wages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for Annual 2024</t>
+    </r>
+  </si>
+  <si>
+    <t>Friday, April 04, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Employment Situation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Wednesday, April 09, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Metropolitan Area Employment and Unemployment (Monthly)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for February 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Thursday, April 10, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Consumer Price Index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Real Earnings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Friday, April 11, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Producer Price Index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Tuesday, April 15, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>U.S. Import and Export Price Indexes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Wednesday, April 16, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>State Job Openings and Labor Turnover</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for February 2025</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Usual Weekly Earnings of Wage and Salary Workers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for First Quarter 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Friday, April 18, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>State Employment and Unemployment (Monthly)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Tuesday, April 22, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>College Enrollment and Work Activity of High School Graduates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for Annual 2024</t>
+    </r>
+  </si>
+  <si>
+    <t>Wednesday, April 23, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Employment Characteristics of Families</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for Annual 2024</t>
+    </r>
+  </si>
+  <si>
+    <t>Tuesday, April 29, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Job Openings and Labor Turnover Survey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Metropolitan Area Employment and Unemployment (Monthly)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for March 2025</t>
+    </r>
+  </si>
+  <si>
+    <t>Wednesday, April 30, 2025</t>
+  </si>
+  <si>
+    <r>
+      <t>Employment Cost Index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> for First Quarter 2025</t>
     </r>
   </si>
 </sst>
@@ -3927,10 +4190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AEC858-1612-40EC-946F-C2E18903E8BB}">
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="E223" sqref="E223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6353,6 +6616,182 @@
         <v>397</v>
       </c>
     </row>
+    <row r="223" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A223" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B223" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C223" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A224" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B224" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A225" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B225" s="4">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C225" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="27" x14ac:dyDescent="0.35">
+      <c r="A226" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B226" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A227" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B227" s="4">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C227" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A228" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B228" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A229" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B229" s="4">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C229" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A230" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B230" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A231" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B231" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C231" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A232" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B232" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="27" x14ac:dyDescent="0.35">
+      <c r="A233" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B233" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C233" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="27" x14ac:dyDescent="0.35">
+      <c r="A234" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B234" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A235" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B235" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A236" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B236" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="27" x14ac:dyDescent="0.35">
+      <c r="A237" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B237" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A238" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B238" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{64AEC858-1612-40EC-946F-C2E18903E8BB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>